<commit_message>
Implemented User Login, SignUp and Admin Login APIs
</commit_message>
<xml_diff>
--- a/data/JobPortalDatabase.xlsx
+++ b/data/JobPortalDatabase.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paramjotsingh/Desktop/JobPortalBackend/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paramjotsingh/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFEFC01B-8DEF-9941-B3BE-2F1D5FDE534B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A010E3-7344-D640-A5BB-52682C8BFF81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="780" windowWidth="34160" windowHeight="19900" activeTab="4" xr2:uid="{5D604037-1A9D-5843-9ABC-114ADD599002}"/>
+    <workbookView xWindow="40" yWindow="780" windowWidth="34160" windowHeight="19900" activeTab="1" xr2:uid="{5D604037-1A9D-5843-9ABC-114ADD599002}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>Email</t>
   </si>
@@ -100,13 +100,35 @@
   </si>
   <si>
     <t>Experience2</t>
+  </si>
+  <si>
+    <t>paramjotsingh966@gmail.com</t>
+  </si>
+  <si>
+    <t>U#00001</t>
+  </si>
+  <si>
+    <t>Paramjot</t>
+  </si>
+  <si>
+    <t>Singh</t>
+  </si>
+  <si>
+    <t>9031398069</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>java,reactJs,networking,android</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -118,6 +140,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -140,14 +170,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -460,14 +493,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5311400-6CFA-5F4B-9B42-E976C131D59F}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="49.33203125" customWidth="1"/>
-    <col min="2" max="2" width="46.83203125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="49.33203125" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="46.83203125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -478,28 +513,39 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>1234</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{DD86BD9D-C55D-C64E-817A-B3B336726EE4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09B30EF7-6740-034B-B554-3754C1991891}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.5" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
-    <col min="4" max="4" width="25.1640625" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" customWidth="1"/>
-    <col min="6" max="6" width="34" customWidth="1"/>
-    <col min="7" max="7" width="54.1640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="19.6640625" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="23.5" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="25.33203125" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="34.5" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="32.5" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="34.0" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="54.1640625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -523,6 +569,29 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -560,32 +629,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9435B3C0-622D-D74C-A082-303FBC3E8782}">
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" customWidth="1"/>
-    <col min="2" max="2" width="29.83203125" customWidth="1"/>
-    <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="5" width="29.6640625" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" customWidth="1"/>
-    <col min="7" max="7" width="28.1640625" customWidth="1"/>
-    <col min="8" max="8" width="24.83203125" customWidth="1"/>
-    <col min="9" max="9" width="28.83203125" customWidth="1"/>
-    <col min="10" max="10" width="25.6640625" customWidth="1"/>
-    <col min="11" max="11" width="30.1640625" customWidth="1"/>
-    <col min="12" max="12" width="26.83203125" customWidth="1"/>
-    <col min="13" max="13" width="29.33203125" customWidth="1"/>
-    <col min="14" max="14" width="26.5" customWidth="1"/>
-    <col min="15" max="15" width="26" customWidth="1"/>
-    <col min="16" max="16" width="26.1640625" customWidth="1"/>
-    <col min="17" max="17" width="26" customWidth="1"/>
-    <col min="18" max="18" width="26.5" customWidth="1"/>
-    <col min="19" max="19" width="24.5" customWidth="1"/>
-    <col min="20" max="20" width="26.1640625" customWidth="1"/>
-    <col min="21" max="21" width="22" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="21.1640625" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="29.83203125" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="29.0" collapsed="false"/>
+    <col min="4" max="5" customWidth="true" width="29.6640625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="27.33203125" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="28.1640625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="24.83203125" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="28.83203125" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="25.6640625" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="30.1640625" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" width="26.83203125" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" width="29.33203125" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" width="26.5" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" width="26.0" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" width="26.1640625" collapsed="false"/>
+    <col min="17" max="17" customWidth="true" width="26.0" collapsed="false"/>
+    <col min="18" max="18" customWidth="true" width="26.5" collapsed="false"/>
+    <col min="19" max="19" customWidth="true" width="24.5" collapsed="false"/>
+    <col min="20" max="20" customWidth="true" width="26.1640625" collapsed="false"/>
+    <col min="21" max="21" customWidth="true" width="22.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added Job entity and some Job APIs
</commit_message>
<xml_diff>
--- a/data/JobPortalDatabase.xlsx
+++ b/data/JobPortalDatabase.xlsx
@@ -3,25 +3,26 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paramjotsingh/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A010E3-7344-D640-A5BB-52682C8BFF81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FC22EB-F452-A342-B30B-C98EAD2D16B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="780" windowWidth="34160" windowHeight="19900" activeTab="1" xr2:uid="{5D604037-1A9D-5843-9ABC-114ADD599002}"/>
+    <workbookView xWindow="40" yWindow="780" windowWidth="34160" windowHeight="19900" activeTab="5" xr2:uid="{5D604037-1A9D-5843-9ABC-114ADD599002}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
     <sheet name="Users" sheetId="2" r:id="rId2"/>
-    <sheet name="Companies" sheetId="3" r:id="rId3"/>
-    <sheet name="Jobs" sheetId="4" r:id="rId4"/>
-    <sheet name="Resume" sheetId="5" r:id="rId5"/>
+    <sheet name="Resume" sheetId="5" r:id="rId3"/>
+    <sheet name="Companies" sheetId="3" r:id="rId4"/>
+    <sheet name="Jobs" sheetId="4" r:id="rId5"/>
+    <sheet name="JobApplications" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>Email</t>
   </si>
@@ -84,18 +85,6 @@
     <t>Link2</t>
   </si>
   <si>
-    <t>Project3</t>
-  </si>
-  <si>
-    <t>Link3</t>
-  </si>
-  <si>
-    <t>Project4</t>
-  </si>
-  <si>
-    <t>Link4</t>
-  </si>
-  <si>
     <t>Experience1</t>
   </si>
   <si>
@@ -121,13 +110,57 @@
   </si>
   <si>
     <t>java,reactJs,networking,android</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Skills</t>
+  </si>
+  <si>
+    <t>CompanyId</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>ImageUrl</t>
+  </si>
+  <si>
+    <t>CompanyDescription</t>
+  </si>
+  <si>
+    <t>JobId</t>
+  </si>
+  <si>
+    <t>RoleTitle</t>
+  </si>
+  <si>
+    <t>RoleDescription</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>RequiredSkills</t>
+  </si>
+  <si>
+    <t>Experience</t>
+  </si>
+  <si>
+    <t>Highest Degree</t>
+  </si>
+  <si>
+    <t>ApplicationStatus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -501,8 +534,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="49.33203125" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="46.83203125" collapsed="false"/>
+    <col min="1" max="1" width="49.33203125" customWidth="1"/>
+    <col min="2" max="2" width="46.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -515,7 +548,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>1234</v>
@@ -533,19 +566,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09B30EF7-6740-034B-B554-3754C1991891}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.6640625" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="23.5" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="25.33203125" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="34.5" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="32.5" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="34.0" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="54.1640625" collapsed="false"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.5" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="34.5" customWidth="1"/>
+    <col min="5" max="5" width="32.5" customWidth="1"/>
+    <col min="6" max="6" width="34" customWidth="1"/>
+    <col min="7" max="7" width="54.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -571,27 +604,27 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G2" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -600,64 +633,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE7AE158-054B-4947-9A9C-33ECBA00D441}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9435B3C0-622D-D74C-A082-303FBC3E8782}">
+  <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB8B4A1-5466-CC48-A629-335591466AFA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9435B3C0-622D-D74C-A082-303FBC3E8782}">
-  <dimension ref="A1:U1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.1640625" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="29.83203125" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="29.0" collapsed="false"/>
-    <col min="4" max="5" customWidth="true" width="29.6640625" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="27.33203125" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="28.1640625" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="24.83203125" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="28.83203125" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="25.6640625" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="30.1640625" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" width="26.83203125" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" width="29.33203125" collapsed="false"/>
-    <col min="14" max="14" customWidth="true" width="26.5" collapsed="false"/>
-    <col min="15" max="15" customWidth="true" width="26.0" collapsed="false"/>
-    <col min="16" max="16" customWidth="true" width="26.1640625" collapsed="false"/>
-    <col min="17" max="17" customWidth="true" width="26.0" collapsed="false"/>
-    <col min="18" max="18" customWidth="true" width="26.5" collapsed="false"/>
-    <col min="19" max="19" customWidth="true" width="24.5" collapsed="false"/>
-    <col min="20" max="20" customWidth="true" width="26.1640625" collapsed="false"/>
-    <col min="21" max="21" customWidth="true" width="22.0" collapsed="false"/>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="5" width="29.6640625" customWidth="1"/>
+    <col min="6" max="9" width="27.33203125" customWidth="1"/>
+    <col min="10" max="10" width="28.83203125" customWidth="1"/>
+    <col min="11" max="11" width="25.6640625" customWidth="1"/>
+    <col min="12" max="12" width="30.1640625" customWidth="1"/>
+    <col min="13" max="13" width="26.83203125" customWidth="1"/>
+    <col min="14" max="14" width="29.33203125" customWidth="1"/>
+    <col min="15" max="15" width="26.5" customWidth="1"/>
+    <col min="16" max="16" width="24.5" customWidth="1"/>
+    <col min="17" max="17" width="26.1640625" customWidth="1"/>
+    <col min="18" max="18" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -677,48 +678,156 @@
         <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1"/>
+      <c r="R1" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE7AE158-054B-4947-9A9C-33ECBA00D441}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+    <col min="2" max="3" width="33.1640625" customWidth="1"/>
+    <col min="4" max="4" width="35.6640625" customWidth="1"/>
+    <col min="5" max="5" width="90" customWidth="1"/>
+    <col min="6" max="7" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB8B4A1-5466-CC48-A629-335591466AFA}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.5" customWidth="1"/>
+    <col min="3" max="3" width="30.5" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" customWidth="1"/>
+    <col min="5" max="5" width="32.1640625" customWidth="1"/>
+    <col min="6" max="6" width="44.83203125" customWidth="1"/>
+    <col min="7" max="7" width="32.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90FA5B83-BD6D-B949-BFEA-972A203D77FB}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="32.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Add Job API
</commit_message>
<xml_diff>
--- a/data/JobPortalDatabase.xlsx
+++ b/data/JobPortalDatabase.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="118">
   <si>
     <t>Email</t>
   </si>
@@ -446,6 +446,12 @@
   </si>
   <si>
     <t>APPLIED</t>
+  </si>
+  <si>
+    <t>aman@gmail.com</t>
+  </si>
+  <si>
+    <t>java,django,cpp,bigData,networking</t>
   </si>
 </sst>
 </file>
@@ -910,7 +916,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09B30EF7-6740-034B-B554-3754C1991891}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -971,6 +977,29 @@
       </c>
       <c r="G2" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed Resume Sheet Headers
</commit_message>
<xml_diff>
--- a/data/JobPortalDatabase.xlsx
+++ b/data/JobPortalDatabase.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paramjotsingh/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437DAD11-73E6-6941-8940-3B41FE7AF3E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C7D33C-0DD6-BA41-A80A-8B63871CD0BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="19500" windowHeight="11500" activeTab="4" xr2:uid="{5D604037-1A9D-5843-9ABC-114ADD599002}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="19500" windowHeight="11500" activeTab="2" xr2:uid="{5D604037-1A9D-5843-9ABC-114ADD599002}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="114">
   <si>
     <t>Email</t>
   </si>
@@ -53,15 +53,6 @@
     <t>Interests</t>
   </si>
   <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>GitHub</t>
-  </si>
-  <si>
-    <t>LinkedIn</t>
-  </si>
-  <si>
     <t>paramjotsingh966@gmail.com</t>
   </si>
   <si>
@@ -83,12 +74,6 @@
     <t>java,reactJs,networking,android</t>
   </si>
   <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Skills</t>
-  </si>
-  <si>
     <t>CompanyId</t>
   </si>
   <si>
@@ -120,9 +105,6 @@
   </si>
   <si>
     <t>Experience</t>
-  </si>
-  <si>
-    <t>Highest Degree</t>
   </si>
   <si>
     <t>ApplicationStatus</t>
@@ -373,112 +355,99 @@
     <t>Kumar</t>
   </si>
   <si>
-    <t>KR Puram, Bangalore</t>
-  </si>
-  <si>
-    <t>amankumar@gmail.com</t>
+    <t>2 yrs</t>
+  </si>
+  <si>
+    <t>U#00002</t>
+  </si>
+  <si>
+    <t>APPLIED</t>
+  </si>
+  <si>
+    <t>aman@gmail.com</t>
+  </si>
+  <si>
+    <t>java,django,cpp,bigData,networking</t>
+  </si>
+  <si>
+    <t>J#00007</t>
+  </si>
+  <si>
+    <t>Full Stack Engineer</t>
+  </si>
+  <si>
+    <t>Full Stack Engineer develops end to end application where they own the project delivery from inception to execution.</t>
+  </si>
+  <si>
+    <t>12 LPA</t>
+  </si>
+  <si>
+    <t>java,reactJs</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>ACTIVE</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>InstitutionName</t>
+  </si>
+  <si>
+    <t>Degree</t>
+  </si>
+  <si>
+    <t>YearOfGraduation</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Responsibilities</t>
+  </si>
+  <si>
+    <t>Paramjot Singh</t>
+  </si>
+  <si>
+    <t>2024-06-05</t>
+  </si>
+  <si>
+    <t>Reva</t>
   </si>
   <si>
     <t>MCA</t>
   </si>
   <si>
-    <t>java, javaScript</t>
-  </si>
-  <si>
-    <t>22 yrs</t>
-  </si>
-  <si>
-    <t>2 yrs</t>
-  </si>
-  <si>
-    <t>https://github.com/LuckySingh1234</t>
-  </si>
-  <si>
-    <t>www.linkedin.com/in/paramjot-singh-lucky</t>
-  </si>
-  <si>
-    <t>U#00002</t>
-  </si>
-  <si>
-    <t>Rahul</t>
-  </si>
-  <si>
-    <t>Reddy</t>
-  </si>
-  <si>
-    <t>Marathalli, Bangalore</t>
-  </si>
-  <si>
-    <t>rahulreddy@gmail.com</t>
-  </si>
-  <si>
-    <t>23 yrs</t>
-  </si>
-  <si>
-    <t>B.Tech</t>
-  </si>
-  <si>
-    <t>U#00003</t>
-  </si>
-  <si>
-    <t>Nitin</t>
-  </si>
-  <si>
-    <t>WhiteField, Bangalore</t>
-  </si>
-  <si>
-    <t>nitinkumar@gmail.com</t>
-  </si>
-  <si>
-    <t>U#00004</t>
-  </si>
-  <si>
-    <t>Raj</t>
-  </si>
-  <si>
-    <t>Varthur, Bangalore</t>
-  </si>
-  <si>
-    <t>rajsingh@gmail.com</t>
-  </si>
-  <si>
-    <t>21 yrs</t>
-  </si>
-  <si>
-    <t>APPLIED</t>
-  </si>
-  <si>
-    <t>aman@gmail.com</t>
-  </si>
-  <si>
-    <t>java,django,cpp,bigData,networking</t>
-  </si>
-  <si>
-    <t>J#00007</t>
-  </si>
-  <si>
-    <t>Full Stack Engineer</t>
-  </si>
-  <si>
-    <t>Full Stack Engineer develops end to end application where they own the project delivery from inception to execution.</t>
-  </si>
-  <si>
-    <t>12 LPA</t>
-  </si>
-  <si>
-    <t>java,reactJs</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>ACTIVE</t>
+    <t>2024</t>
+  </si>
+  <si>
+    <t>Abc</t>
+  </si>
+  <si>
+    <t>Intern</t>
+  </si>
+  <si>
+    <t>3 Months</t>
+  </si>
+  <si>
+    <t>Frontend
+Backend</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="10">
     <font>
       <sz val="12"/>
@@ -566,7 +535,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -577,12 +546,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -906,8 +869,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="49.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="46.83203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="49.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="46.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -920,7 +883,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>1234</v>
@@ -944,13 +907,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="34.5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.5" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="54.1640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.5" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="34.5" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="32.5" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="54.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -978,48 +941,48 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
         <v>89</v>
-      </c>
-      <c r="C3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1029,23 +992,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9435B3C0-622D-D74C-A082-303FBC3E8782}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.83203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="29.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="9" width="27.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="34.6640625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="44.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="24.5" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.1640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.83203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="6" max="9" customWidth="true" width="27.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="34.6640625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="44.6640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="24.5" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -1053,213 +1016,81 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>98</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" s="1"/>
-    </row>
-    <row r="2" spans="1:13" ht="17">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D2">
-        <v>8852332525</v>
-      </c>
       <c r="E2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>92</v>
+        <v>107</v>
+      </c>
+      <c r="F2" t="s">
+        <v>108</v>
       </c>
       <c r="G2" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="H2" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="I2" t="s">
-        <v>94</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="L2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="17.5" customHeight="1">
-      <c r="A3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3">
-        <v>9835445623</v>
-      </c>
-      <c r="E3" t="s">
-        <v>102</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G3" t="s">
-        <v>104</v>
-      </c>
-      <c r="H3" t="s">
-        <v>105</v>
-      </c>
-      <c r="I3" t="s">
-        <v>72</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="L3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4">
-        <v>7899256605</v>
-      </c>
-      <c r="E4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G4" t="s">
-        <v>95</v>
-      </c>
-      <c r="H4" t="s">
-        <v>93</v>
-      </c>
-      <c r="I4" t="s">
-        <v>88</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="L4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B5" t="s">
         <v>111</v>
       </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5">
-        <v>9934565220</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="J2" t="s">
         <v>112</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="K2" t="s">
         <v>113</v>
       </c>
-      <c r="G5" t="s">
-        <v>114</v>
-      </c>
-      <c r="H5" t="s">
-        <v>105</v>
-      </c>
-      <c r="I5" t="s">
-        <v>83</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="L5" t="s">
-        <v>96</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{B431C306-E9A5-4DCB-87F3-CF91D9DE59E5}"/>
-    <hyperlink ref="J2" r:id="rId2" xr:uid="{46FBDC8C-E2A0-44B3-AE12-5AA6F739B472}"/>
-    <hyperlink ref="F3" r:id="rId3" xr:uid="{56E904FF-E84C-4A5A-9065-8068C2125CD5}"/>
-    <hyperlink ref="K2" r:id="rId4" xr:uid="{3C04BFF7-B991-4193-8948-960B56C89F23}"/>
-    <hyperlink ref="J3" r:id="rId5" xr:uid="{79377C4F-5F12-4689-BA9C-A63BE7BFB7D7}"/>
-    <hyperlink ref="F4" r:id="rId6" xr:uid="{59829561-86BF-485C-86D9-EABFFD19C739}"/>
-    <hyperlink ref="J4" r:id="rId7" xr:uid="{32837B42-E704-4661-A369-7663BD799AA6}"/>
-    <hyperlink ref="F5" r:id="rId8" xr:uid="{E4A4E46C-6EF9-49AD-89EE-099BD05622B3}"/>
-    <hyperlink ref="J5" r:id="rId9" xr:uid="{E1B710A9-8B66-4A29-8906-2F0A8BA36EAD}"/>
-    <hyperlink ref="K4" r:id="rId10" xr:uid="{8DF87A08-8CEB-458D-851F-2FCE09463825}"/>
-    <hyperlink ref="K5" r:id="rId11" xr:uid="{F134FF9A-939E-421E-A79B-D9F275E487A1}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE7AE158-054B-4947-9A9C-33ECBA00D441}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
@@ -1267,131 +1098,131 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="25.1640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.1640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="55.1640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="35.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="154.5" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="10.83203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="25.1640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.1640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="55.1640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="154.5" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" width="10.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
         <v>36</v>
-      </c>
-      <c r="B4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="19.75" customHeight="1">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1404,227 +1235,227 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB8B4A1-5466-CC48-A629-335591466AFA}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="46.83203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="71" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.1640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="44.83203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="32.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="25.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.5" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="46.83203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="71.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="32.1640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="44.83203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="32.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="H2" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H3" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" t="s">
         <v>68</v>
       </c>
-      <c r="G4" t="s">
-        <v>74</v>
-      </c>
       <c r="H4" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="H5" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" t="s">
         <v>75</v>
       </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" t="s">
-        <v>81</v>
-      </c>
       <c r="E6" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F6" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H6" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F7" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="H7" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="E8" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="F8" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="G8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" t="s">
         <v>96</v>
-      </c>
-      <c r="H8" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1642,53 +1473,53 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="22.5" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.1640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.5" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="32.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added My Applications API
</commit_message>
<xml_diff>
--- a/data/JobPortalDatabase.xlsx
+++ b/data/JobPortalDatabase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paramjotsingh/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C7D33C-0DD6-BA41-A80A-8B63871CD0BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F441E77F-02FD-8E43-920B-917878CA4281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="19500" windowHeight="11500" activeTab="2" xr2:uid="{5D604037-1A9D-5843-9ABC-114ADD599002}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="19500" windowHeight="11500" activeTab="5" xr2:uid="{5D604037-1A9D-5843-9ABC-114ADD599002}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="115">
   <si>
     <t>Email</t>
   </si>
@@ -441,6 +441,9 @@
   <si>
     <t>Frontend
 Backend</t>
+  </si>
+  <si>
+    <t>ACCEPTED</t>
   </si>
 </sst>
 </file>
@@ -994,7 +997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9435B3C0-622D-D74C-A082-303FBC3E8782}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1048,7 +1051,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1467,8 +1470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90FA5B83-BD6D-B949-BFEA-972A203D77FB}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
@@ -1497,7 +1500,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:3">

</xml_diff>

<commit_message>
Added Fetch Resume API
</commit_message>
<xml_diff>
--- a/data/JobPortalDatabase.xlsx
+++ b/data/JobPortalDatabase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paramjotsingh/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F441E77F-02FD-8E43-920B-917878CA4281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECC8EB6-E1B4-F343-A962-0526DEC13258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="19500" windowHeight="11500" activeTab="5" xr2:uid="{5D604037-1A9D-5843-9ABC-114ADD599002}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="19500" windowHeight="11500" activeTab="2" xr2:uid="{5D604037-1A9D-5843-9ABC-114ADD599002}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="122">
   <si>
     <t>Email</t>
   </si>
@@ -418,32 +418,60 @@
     <t>Paramjot Singh</t>
   </si>
   <si>
-    <t>2024-06-05</t>
-  </si>
-  <si>
-    <t>Reva</t>
-  </si>
-  <si>
     <t>MCA</t>
   </si>
   <si>
     <t>2024</t>
   </si>
   <si>
-    <t>Abc</t>
+    <t>3 Months</t>
+  </si>
+  <si>
+    <t>ACCEPTED</t>
+  </si>
+  <si>
+    <t>REJECTED</t>
+  </si>
+  <si>
+    <t>Xploria</t>
+  </si>
+  <si>
+    <t>Frontend
+HTML
+CSS
+JavaScript
+Backend
+Java
+Apache Tomcat</t>
+  </si>
+  <si>
+    <t>1997-01-26</t>
+  </si>
+  <si>
+    <t>Reva University</t>
+  </si>
+  <si>
+    <t>SDE Internship</t>
+  </si>
+  <si>
+    <t>6 Months</t>
+  </si>
+  <si>
+    <t>Aman Kumar</t>
+  </si>
+  <si>
+    <t>1998-02-14</t>
+  </si>
+  <si>
+    <t>BCA</t>
   </si>
   <si>
     <t>Intern</t>
   </si>
   <si>
-    <t>3 Months</t>
-  </si>
-  <si>
     <t>Frontend
-Backend</t>
-  </si>
-  <si>
-    <t>ACCEPTED</t>
+React Js
+Angular Js</t>
   </si>
 </sst>
 </file>
@@ -995,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9435B3C0-622D-D74C-A082-303FBC3E8782}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
@@ -1009,7 +1037,7 @@
     <col min="4" max="5" customWidth="true" width="29.6640625" collapsed="true"/>
     <col min="6" max="9" customWidth="true" width="27.33203125" collapsed="true"/>
     <col min="10" max="10" customWidth="true" width="34.6640625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="44.6640625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="55.1640625" collapsed="true"/>
     <col min="12" max="12" customWidth="true" width="24.5" collapsed="true"/>
     <col min="13" max="13" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
@@ -1059,31 +1087,66 @@
         <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" t="s">
         <v>107</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I2" t="s">
+        <v>115</v>
+      </c>
+      <c r="J2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" t="s">
+        <v>120</v>
+      </c>
+      <c r="J3" t="s">
         <v>108</v>
       </c>
-      <c r="G2" t="s">
-        <v>109</v>
-      </c>
-      <c r="H2" t="s">
-        <v>110</v>
-      </c>
-      <c r="I2" t="s">
-        <v>111</v>
-      </c>
-      <c r="J2" t="s">
-        <v>112</v>
-      </c>
-      <c r="K2" t="s">
-        <v>113</v>
+      <c r="K3" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1470,7 +1533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90FA5B83-BD6D-B949-BFEA-972A203D77FB}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1500,7 +1563,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1522,7 +1585,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>